<commit_message>
Project CAP Financial is saved. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/CAP Financial/rules/config_financial_base.xlsx
+++ b/DESIGN/rules/CAP Financial/rules/config_financial_base.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="22">
   <si>
     <t>Fica Type</t>
   </si>
@@ -83,6 +83,15 @@
   </si>
   <si>
     <t>Rate</t>
+  </si>
+  <si>
+    <t>properties</t>
+  </si>
+  <si>
+    <t>origin</t>
+  </si>
+  <si>
+    <t>Deviation</t>
   </si>
 </sst>
 </file>
@@ -207,7 +216,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -445,12 +454,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -510,6 +561,41 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="true"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="true"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="true"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,198 +817,216 @@
       <c r="E2" s="21"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="B3" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="39"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="20">
-        <v>2025</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E4" s="8">
-        <v>200000</v>
+      <c r="B4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="20"/>
-      <c r="C5" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E5" s="10"/>
+      <c r="B5" s="20" t="n">
+        <v>2025.0</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E5" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="20"/>
-      <c r="C6" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="11">
-        <v>6.2</v>
-      </c>
-      <c r="E6" s="12">
-        <v>168600</v>
-      </c>
+      <c r="B6" s="36"/>
+      <c r="C6" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="20">
-        <v>2024</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E7" s="8">
-        <v>200000</v>
+      <c r="B7" s="35"/>
+      <c r="C7" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="11" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E7" s="12" t="n">
+        <v>168600.0</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="20"/>
-      <c r="C8" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E8" s="10"/>
+      <c r="B8" s="20" t="n">
+        <v>2024.0</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E8" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="20"/>
-      <c r="C9" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="11">
-        <v>6.2</v>
-      </c>
-      <c r="E9" s="12">
-        <v>168600</v>
-      </c>
+      <c r="B9" s="34"/>
+      <c r="C9" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E9" s="10"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="20">
-        <v>2023</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E10" s="8">
-        <v>200000</v>
+      <c r="B10" s="33"/>
+      <c r="C10" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="11" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E10" s="12" t="n">
+        <v>168600.0</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="20"/>
-      <c r="C11" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E11" s="10"/>
+      <c r="B11" s="20" t="n">
+        <v>2023.0</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E11" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="20"/>
-      <c r="C12" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="13">
-        <v>6.2</v>
-      </c>
-      <c r="E12" s="14">
-        <v>152000</v>
-      </c>
+      <c r="B12" s="32"/>
+      <c r="C12" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E12" s="10"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="20">
-        <v>2022</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E13" s="8">
-        <v>200000</v>
+      <c r="B13" s="31"/>
+      <c r="C13" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="13" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E13" s="14" t="n">
+        <v>152000.0</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="20"/>
-      <c r="C14" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E14" s="10"/>
+      <c r="B14" s="20" t="n">
+        <v>2022.0</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E14" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="20"/>
-      <c r="C15" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="11">
-        <v>6.2</v>
-      </c>
-      <c r="E15" s="12">
-        <v>147000</v>
-      </c>
+      <c r="B15" s="30"/>
+      <c r="C15" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E15" s="10"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="20">
-        <v>2021</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E16" s="8">
-        <v>200000</v>
+      <c r="B16" s="29"/>
+      <c r="C16" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="11" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E16" s="12" t="n">
+        <v>147000.0</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="20"/>
-      <c r="C17" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E17" s="10"/>
+      <c r="B17" s="20" t="n">
+        <v>2021.0</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E17" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="20"/>
-      <c r="C18" s="18" t="s">
+      <c r="B18" s="28"/>
+      <c r="C18" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19">
+      <c r="B19" s="27"/>
+      <c r="C19" t="s" s="18">
         <v>2</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D19" t="s" s="11">
         <v>3</v>
       </c>
-      <c r="E18" s="12">
-        <v>142800</v>
-      </c>
+      <c r="E19" t="n" s="12">
+        <v>142800.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" s="26"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="23"/>
     </row>
     <row r="1047484" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1047485" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1988,13 +2092,13 @@
     <row r="1048545" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1048546" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B16:B18"/>
+  <mergeCells count="11">
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B5:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
changes of user Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/CAP Financial/rules/config_financial_base.xlsx
+++ b/DESIGN/rules/CAP Financial/rules/config_financial_base.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="23">
   <si>
     <t>Fica Type</t>
   </si>
@@ -867,7 +867,7 @@
         <v>14</v>
       </c>
       <c r="D6" s="9" t="n">
-        <v>1.45</v>
+        <v>1.453</v>
       </c>
       <c r="E6" s="10"/>
     </row>

</xml_diff>

<commit_message>
admin added origin prop Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/CAP Financial/rules/config_financial_base.xlsx
+++ b/DESIGN/rules/CAP Financial/rules/config_financial_base.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="22">
   <si>
     <t>Fica Type</t>
   </si>
@@ -83,6 +83,15 @@
   </si>
   <si>
     <t>Rate</t>
+  </si>
+  <si>
+    <t>properties</t>
+  </si>
+  <si>
+    <t>origin</t>
+  </si>
+  <si>
+    <t>Deviation</t>
   </si>
 </sst>
 </file>
@@ -207,7 +216,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -445,12 +454,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -510,6 +561,41 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="true"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="true"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="true"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,198 +817,216 @@
       <c r="E2" s="21"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="B3" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="39"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="20">
-        <v>2025</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E4" s="8">
-        <v>200000</v>
+      <c r="B4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="20"/>
-      <c r="C5" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E5" s="10"/>
+      <c r="B5" s="20" t="n">
+        <v>2025.0</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E5" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="20"/>
-      <c r="C6" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="11">
-        <v>6.2</v>
-      </c>
-      <c r="E6" s="12">
-        <v>168600</v>
-      </c>
+      <c r="B6" s="36"/>
+      <c r="C6" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="20">
-        <v>2024</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E7" s="8">
-        <v>200000</v>
+      <c r="B7" s="35"/>
+      <c r="C7" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="11" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E7" s="12" t="n">
+        <v>168600.0</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="20"/>
-      <c r="C8" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E8" s="10"/>
+      <c r="B8" s="20" t="n">
+        <v>2024.0</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E8" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="20"/>
-      <c r="C9" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="11">
-        <v>6.2</v>
-      </c>
-      <c r="E9" s="12">
-        <v>168600</v>
-      </c>
+      <c r="B9" s="34"/>
+      <c r="C9" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E9" s="10"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="20">
-        <v>2023</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E10" s="8">
-        <v>200000</v>
+      <c r="B10" s="33"/>
+      <c r="C10" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="11" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E10" s="12" t="n">
+        <v>168600.0</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="20"/>
-      <c r="C11" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E11" s="10"/>
+      <c r="B11" s="20" t="n">
+        <v>2023.0</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E11" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="20"/>
-      <c r="C12" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="13">
-        <v>6.2</v>
-      </c>
-      <c r="E12" s="14">
-        <v>152000</v>
-      </c>
+      <c r="B12" s="32"/>
+      <c r="C12" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E12" s="10"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="20">
-        <v>2022</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E13" s="8">
-        <v>200000</v>
+      <c r="B13" s="31"/>
+      <c r="C13" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="13" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E13" s="14" t="n">
+        <v>152000.0</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="20"/>
-      <c r="C14" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E14" s="10"/>
+      <c r="B14" s="20" t="n">
+        <v>2022.0</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E14" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="20"/>
-      <c r="C15" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="11">
-        <v>6.2</v>
-      </c>
-      <c r="E15" s="12">
-        <v>147000</v>
-      </c>
+      <c r="B15" s="30"/>
+      <c r="C15" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E15" s="10"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="20">
-        <v>2021</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E16" s="8">
-        <v>200000</v>
+      <c r="B16" s="29"/>
+      <c r="C16" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="11" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E16" s="12" t="n">
+        <v>147000.0</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="20"/>
-      <c r="C17" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E17" s="10"/>
+      <c r="B17" s="20" t="n">
+        <v>2021.0</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E17" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="20"/>
-      <c r="C18" s="18" t="s">
+      <c r="B18" s="28"/>
+      <c r="C18" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19">
+      <c r="B19" s="27"/>
+      <c r="C19" t="s" s="18">
         <v>2</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D19" t="s" s="11">
         <v>3</v>
       </c>
-      <c r="E18" s="12">
-        <v>142800</v>
-      </c>
+      <c r="E19" t="n" s="12">
+        <v>142800.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" s="26"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="23"/>
     </row>
     <row r="1047484" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1047485" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1988,13 +2092,13 @@
     <row r="1048545" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1048546" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B16:B18"/>
+  <mergeCells count="11">
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B5:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
saving properties Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/CAP Financial/rules/config_financial_base.xlsx
+++ b/DESIGN/rules/CAP Financial/rules/config_financial_base.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="22">
   <si>
     <t>Fica Type</t>
   </si>
@@ -83,6 +83,15 @@
   </si>
   <si>
     <t>Rate</t>
+  </si>
+  <si>
+    <t>properties</t>
+  </si>
+  <si>
+    <t>origin</t>
+  </si>
+  <si>
+    <t>Deviation</t>
   </si>
 </sst>
 </file>
@@ -207,7 +216,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -445,12 +454,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -510,6 +561,41 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="true"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="true"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="true"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,198 +817,216 @@
       <c r="E2" s="21"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="B3" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="39"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="20">
-        <v>2025</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E4" s="8">
-        <v>200000</v>
+      <c r="B4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="20"/>
-      <c r="C5" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E5" s="10"/>
+      <c r="B5" s="20" t="n">
+        <v>2025.0</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E5" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="20"/>
-      <c r="C6" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="11">
-        <v>6.2</v>
-      </c>
-      <c r="E6" s="12">
-        <v>168600</v>
-      </c>
+      <c r="B6" s="36"/>
+      <c r="C6" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="20">
-        <v>2024</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E7" s="8">
-        <v>200000</v>
+      <c r="B7" s="35"/>
+      <c r="C7" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="11" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E7" s="12" t="n">
+        <v>168600.0</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="20"/>
-      <c r="C8" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E8" s="10"/>
+      <c r="B8" s="20" t="n">
+        <v>2024.0</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E8" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="20"/>
-      <c r="C9" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="11">
-        <v>6.2</v>
-      </c>
-      <c r="E9" s="12">
-        <v>168600</v>
-      </c>
+      <c r="B9" s="34"/>
+      <c r="C9" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E9" s="10"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="20">
-        <v>2023</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E10" s="8">
-        <v>200000</v>
+      <c r="B10" s="33"/>
+      <c r="C10" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="11" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E10" s="12" t="n">
+        <v>168600.0</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="20"/>
-      <c r="C11" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E11" s="10"/>
+      <c r="B11" s="20" t="n">
+        <v>2023.0</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E11" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="20"/>
-      <c r="C12" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="13">
-        <v>6.2</v>
-      </c>
-      <c r="E12" s="14">
-        <v>152000</v>
-      </c>
+      <c r="B12" s="32"/>
+      <c r="C12" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E12" s="10"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="20">
-        <v>2022</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E13" s="8">
-        <v>200000</v>
+      <c r="B13" s="31"/>
+      <c r="C13" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="13" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E13" s="14" t="n">
+        <v>152000.0</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="20"/>
-      <c r="C14" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E14" s="10"/>
+      <c r="B14" s="20" t="n">
+        <v>2022.0</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E14" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="20"/>
-      <c r="C15" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="11">
-        <v>6.2</v>
-      </c>
-      <c r="E15" s="12">
-        <v>147000</v>
-      </c>
+      <c r="B15" s="30"/>
+      <c r="C15" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E15" s="10"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="20">
-        <v>2021</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E16" s="8">
-        <v>200000</v>
+      <c r="B16" s="29"/>
+      <c r="C16" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="11" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E16" s="12" t="n">
+        <v>147000.0</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="20"/>
-      <c r="C17" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E17" s="10"/>
+      <c r="B17" s="20" t="n">
+        <v>2021.0</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E17" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="20"/>
-      <c r="C18" s="18" t="s">
+      <c r="B18" s="28"/>
+      <c r="C18" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19">
+      <c r="B19" s="27"/>
+      <c r="C19" t="s" s="18">
         <v>2</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D19" t="s" s="11">
         <v>3</v>
       </c>
-      <c r="E18" s="12">
-        <v>142800</v>
-      </c>
+      <c r="E19" t="n" s="12">
+        <v>142800.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" s="26"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="23"/>
     </row>
     <row r="1047484" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1047485" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1988,13 +2092,13 @@
     <row r="1048545" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1048546" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B16:B18"/>
+  <mergeCells count="11">
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B5:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
saved origin property Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/CAP Financial/rules/config_financial_base.xlsx
+++ b/DESIGN/rules/CAP Financial/rules/config_financial_base.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="22">
   <si>
     <t>Fica Type</t>
   </si>
@@ -83,6 +83,15 @@
   </si>
   <si>
     <t>Rate</t>
+  </si>
+  <si>
+    <t>properties</t>
+  </si>
+  <si>
+    <t>origin</t>
+  </si>
+  <si>
+    <t>Deviation</t>
   </si>
 </sst>
 </file>
@@ -207,7 +216,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -445,12 +454,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -510,6 +561,41 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="true"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="true"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="true"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,198 +817,216 @@
       <c r="E2" s="21"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="B3" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="39"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="20">
-        <v>2025</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E4" s="8">
-        <v>200000</v>
+      <c r="B4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="20"/>
-      <c r="C5" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E5" s="10"/>
+      <c r="B5" s="20" t="n">
+        <v>2025.0</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E5" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="20"/>
-      <c r="C6" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="11">
-        <v>6.2</v>
-      </c>
-      <c r="E6" s="12">
-        <v>168600</v>
-      </c>
+      <c r="B6" s="36"/>
+      <c r="C6" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="20">
-        <v>2024</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E7" s="8">
-        <v>200000</v>
+      <c r="B7" s="35"/>
+      <c r="C7" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="11" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E7" s="12" t="n">
+        <v>168600.0</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="20"/>
-      <c r="C8" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E8" s="10"/>
+      <c r="B8" s="20" t="n">
+        <v>2024.0</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E8" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="20"/>
-      <c r="C9" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="11">
-        <v>6.2</v>
-      </c>
-      <c r="E9" s="12">
-        <v>168600</v>
-      </c>
+      <c r="B9" s="34"/>
+      <c r="C9" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E9" s="10"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="20">
-        <v>2023</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E10" s="8">
-        <v>200000</v>
+      <c r="B10" s="33"/>
+      <c r="C10" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="11" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E10" s="12" t="n">
+        <v>168600.0</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="20"/>
-      <c r="C11" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E11" s="10"/>
+      <c r="B11" s="20" t="n">
+        <v>2023.0</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E11" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="20"/>
-      <c r="C12" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="13">
-        <v>6.2</v>
-      </c>
-      <c r="E12" s="14">
-        <v>152000</v>
-      </c>
+      <c r="B12" s="32"/>
+      <c r="C12" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E12" s="10"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="20">
-        <v>2022</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E13" s="8">
-        <v>200000</v>
+      <c r="B13" s="31"/>
+      <c r="C13" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="13" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E13" s="14" t="n">
+        <v>152000.0</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="20"/>
-      <c r="C14" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E14" s="10"/>
+      <c r="B14" s="20" t="n">
+        <v>2022.0</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E14" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="20"/>
-      <c r="C15" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="11">
-        <v>6.2</v>
-      </c>
-      <c r="E15" s="12">
-        <v>147000</v>
-      </c>
+      <c r="B15" s="30"/>
+      <c r="C15" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E15" s="10"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="20">
-        <v>2021</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E16" s="8">
-        <v>200000</v>
+      <c r="B16" s="29"/>
+      <c r="C16" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="11" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E16" s="12" t="n">
+        <v>147000.0</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="20"/>
-      <c r="C17" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E17" s="10"/>
+      <c r="B17" s="20" t="n">
+        <v>2021.0</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E17" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="20"/>
-      <c r="C18" s="18" t="s">
+      <c r="B18" s="28"/>
+      <c r="C18" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19">
+      <c r="B19" s="27"/>
+      <c r="C19" t="s" s="18">
         <v>2</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D19" t="s" s="11">
         <v>3</v>
       </c>
-      <c r="E18" s="12">
-        <v>142800</v>
-      </c>
+      <c r="E19" t="n" s="12">
+        <v>142800.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" s="26"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="23"/>
     </row>
     <row r="1047484" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1047485" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1988,13 +2092,13 @@
     <row r="1048545" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1048546" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B16:B18"/>
+  <mergeCells count="11">
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B5:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
adding year from admin Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/CAP Financial/rules/config_financial_base.xlsx
+++ b/DESIGN/rules/CAP Financial/rules/config_financial_base.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="23">
   <si>
     <t>Fica Type</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>Deviation</t>
+  </si>
+  <si>
+    <t>SmartRules PaymentToolsFicaDetails FicaTaxRates(PaymentToolsFicaInput input)</t>
   </si>
 </sst>
 </file>
@@ -810,7 +813,7 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B2" s="21" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C2" s="21"/>
       <c r="D2" s="21"/>
@@ -844,7 +847,7 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="20" t="n">
-        <v>2025.0</v>
+        <v>2026.0</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>13</v>
@@ -857,7 +860,9 @@
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="36"/>
+      <c r="B6" s="36" t="n">
+        <v>2026.0</v>
+      </c>
       <c r="C6" s="17" t="s">
         <v>14</v>
       </c>
@@ -867,7 +872,9 @@
       <c r="E6" s="10"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="35"/>
+      <c r="B7" s="35" t="n">
+        <v>2026.0</v>
+      </c>
       <c r="C7" s="18" t="s">
         <v>2</v>
       </c>
@@ -880,7 +887,7 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" s="20" t="n">
-        <v>2024.0</v>
+        <v>2025.0</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>13</v>
@@ -893,7 +900,9 @@
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="34"/>
+      <c r="B9" s="34" t="n">
+        <v>2025.0</v>
+      </c>
       <c r="C9" s="17" t="s">
         <v>14</v>
       </c>
@@ -903,7 +912,9 @@
       <c r="E9" s="10"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="33"/>
+      <c r="B10" s="33" t="n">
+        <v>2025.0</v>
+      </c>
       <c r="C10" s="18" t="s">
         <v>2</v>
       </c>
@@ -916,7 +927,7 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B11" s="20" t="n">
-        <v>2023.0</v>
+        <v>2024.0</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>13</v>
@@ -929,7 +940,9 @@
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="32"/>
+      <c r="B12" s="32" t="n">
+        <v>2024.0</v>
+      </c>
       <c r="C12" s="17" t="s">
         <v>14</v>
       </c>
@@ -939,7 +952,9 @@
       <c r="E12" s="10"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="31"/>
+      <c r="B13" s="31" t="n">
+        <v>2024.0</v>
+      </c>
       <c r="C13" s="19" t="s">
         <v>2</v>
       </c>
@@ -947,12 +962,12 @@
         <v>6.2</v>
       </c>
       <c r="E13" s="14" t="n">
-        <v>152000.0</v>
+        <v>168600.0</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B14" s="20" t="n">
-        <v>2022.0</v>
+        <v>2023.0</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>13</v>
@@ -965,7 +980,9 @@
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="30"/>
+      <c r="B15" s="30" t="n">
+        <v>2023.0</v>
+      </c>
       <c r="C15" s="17" t="s">
         <v>14</v>
       </c>
@@ -975,7 +992,9 @@
       <c r="E15" s="10"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="29"/>
+      <c r="B16" s="29" t="n">
+        <v>2023.0</v>
+      </c>
       <c r="C16" s="18" t="s">
         <v>2</v>
       </c>
@@ -983,12 +1002,12 @@
         <v>6.2</v>
       </c>
       <c r="E16" s="12" t="n">
-        <v>147000.0</v>
+        <v>152000.0</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="20" t="n">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>13</v>
@@ -1001,7 +1020,9 @@
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="28"/>
+      <c r="B18" s="28" t="n">
+        <v>2022.0</v>
+      </c>
       <c r="C18" s="17" t="s">
         <v>14</v>
       </c>
@@ -1011,22 +1032,64 @@
       <c r="E18" s="10"/>
     </row>
     <row r="19">
-      <c r="B19" s="27"/>
-      <c r="C19" t="s" s="18">
+      <c r="B19" s="27" t="n">
+        <v>2022.0</v>
+      </c>
+      <c r="C19" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D19" t="s" s="11">
-        <v>3</v>
+      <c r="D19" t="n" s="11">
+        <v>6.2</v>
       </c>
       <c r="E19" t="n" s="12">
-        <v>142800.0</v>
+        <v>147000.0</v>
       </c>
     </row>
     <row r="20">
-      <c r="B20" s="26"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="23"/>
+      <c r="B20" t="n" s="5">
+        <v>2021.0</v>
+      </c>
+      <c r="C20" t="s" s="5">
+        <v>13</v>
+      </c>
+      <c r="D20" t="n" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="E20" t="n" s="5">
+        <v>200000.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="n" s="5">
+        <v>2021.0</v>
+      </c>
+      <c r="C21" t="s" s="5">
+        <v>14</v>
+      </c>
+      <c r="D21" t="n" s="5">
+        <v>1.45</v>
+      </c>
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22">
+      <c r="B22" t="n" s="5">
+        <v>2021.0</v>
+      </c>
+      <c r="C22" t="s" s="5">
+        <v>2</v>
+      </c>
+      <c r="D22" t="n" s="5">
+        <v>6.2</v>
+      </c>
+      <c r="E22" t="n" s="5">
+        <v>142800.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" s="5"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
     </row>
     <row r="1047484" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1047485" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
properties adding Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/CAP Financial/rules/config_financial_base.xlsx
+++ b/DESIGN/rules/CAP Financial/rules/config_financial_base.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="22">
   <si>
     <t>Fica Type</t>
   </si>
@@ -83,6 +83,15 @@
   </si>
   <si>
     <t>Rate</t>
+  </si>
+  <si>
+    <t>properties</t>
+  </si>
+  <si>
+    <t>origin</t>
+  </si>
+  <si>
+    <t>Deviation</t>
   </si>
 </sst>
 </file>
@@ -207,7 +216,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -445,12 +454,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -510,6 +561,41 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="true"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="true"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="true"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,198 +817,216 @@
       <c r="E2" s="21"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="B3" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="39"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="20">
-        <v>2025</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E4" s="8">
-        <v>200000</v>
+      <c r="B4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="20"/>
-      <c r="C5" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E5" s="10"/>
+      <c r="B5" s="20" t="n">
+        <v>2025.0</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E5" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="20"/>
-      <c r="C6" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="11">
-        <v>6.2</v>
-      </c>
-      <c r="E6" s="12">
-        <v>168600</v>
-      </c>
+      <c r="B6" s="36"/>
+      <c r="C6" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="20">
-        <v>2024</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E7" s="8">
-        <v>200000</v>
+      <c r="B7" s="35"/>
+      <c r="C7" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="11" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E7" s="12" t="n">
+        <v>168600.0</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="20"/>
-      <c r="C8" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E8" s="10"/>
+      <c r="B8" s="20" t="n">
+        <v>2024.0</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E8" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="20"/>
-      <c r="C9" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="11">
-        <v>6.2</v>
-      </c>
-      <c r="E9" s="12">
-        <v>168600</v>
-      </c>
+      <c r="B9" s="34"/>
+      <c r="C9" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E9" s="10"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="20">
-        <v>2023</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E10" s="8">
-        <v>200000</v>
+      <c r="B10" s="33"/>
+      <c r="C10" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="11" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E10" s="12" t="n">
+        <v>168600.0</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="20"/>
-      <c r="C11" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E11" s="10"/>
+      <c r="B11" s="20" t="n">
+        <v>2023.0</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E11" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="20"/>
-      <c r="C12" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="13">
-        <v>6.2</v>
-      </c>
-      <c r="E12" s="14">
-        <v>152000</v>
-      </c>
+      <c r="B12" s="32"/>
+      <c r="C12" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E12" s="10"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="20">
-        <v>2022</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E13" s="8">
-        <v>200000</v>
+      <c r="B13" s="31"/>
+      <c r="C13" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="13" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E13" s="14" t="n">
+        <v>152000.0</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="20"/>
-      <c r="C14" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E14" s="10"/>
+      <c r="B14" s="20" t="n">
+        <v>2022.0</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E14" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="20"/>
-      <c r="C15" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="11">
-        <v>6.2</v>
-      </c>
-      <c r="E15" s="12">
-        <v>147000</v>
-      </c>
+      <c r="B15" s="30"/>
+      <c r="C15" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E15" s="10"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="20">
-        <v>2021</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E16" s="8">
-        <v>200000</v>
+      <c r="B16" s="29"/>
+      <c r="C16" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="11" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E16" s="12" t="n">
+        <v>147000.0</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="20"/>
-      <c r="C17" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E17" s="10"/>
+      <c r="B17" s="20" t="n">
+        <v>2021.0</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E17" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="20"/>
-      <c r="C18" s="18" t="s">
+      <c r="B18" s="28"/>
+      <c r="C18" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19">
+      <c r="B19" s="27"/>
+      <c r="C19" t="s" s="18">
         <v>2</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D19" t="s" s="11">
         <v>3</v>
       </c>
-      <c r="E18" s="12">
-        <v>142800</v>
-      </c>
+      <c r="E19" t="n" s="12">
+        <v>142800.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" s="26"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="23"/>
     </row>
     <row r="1047484" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1047485" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1988,13 +2092,13 @@
     <row r="1048545" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1048546" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B16:B18"/>
+  <mergeCells count="11">
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B5:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
adding properties Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/CAP Financial/rules/config_financial_base.xlsx
+++ b/DESIGN/rules/CAP Financial/rules/config_financial_base.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="22">
   <si>
     <t>Fica Type</t>
   </si>
@@ -83,6 +83,15 @@
   </si>
   <si>
     <t>Rate</t>
+  </si>
+  <si>
+    <t>properties</t>
+  </si>
+  <si>
+    <t>origin</t>
+  </si>
+  <si>
+    <t>Deviation</t>
   </si>
 </sst>
 </file>
@@ -207,7 +216,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -445,12 +454,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -510,6 +561,41 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="true"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="true"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="true"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,198 +817,216 @@
       <c r="E2" s="21"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="B3" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="39"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="20">
-        <v>2025</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E4" s="8">
-        <v>200000</v>
+      <c r="B4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="20"/>
-      <c r="C5" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E5" s="10"/>
+      <c r="B5" s="20" t="n">
+        <v>2025.0</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E5" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="20"/>
-      <c r="C6" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="11">
-        <v>6.2</v>
-      </c>
-      <c r="E6" s="12">
-        <v>168600</v>
-      </c>
+      <c r="B6" s="36"/>
+      <c r="C6" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="20">
-        <v>2024</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E7" s="8">
-        <v>200000</v>
+      <c r="B7" s="35"/>
+      <c r="C7" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="11" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E7" s="12" t="n">
+        <v>168600.0</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="20"/>
-      <c r="C8" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E8" s="10"/>
+      <c r="B8" s="20" t="n">
+        <v>2024.0</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E8" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="20"/>
-      <c r="C9" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="11">
-        <v>6.2</v>
-      </c>
-      <c r="E9" s="12">
-        <v>168600</v>
-      </c>
+      <c r="B9" s="34"/>
+      <c r="C9" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E9" s="10"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="20">
-        <v>2023</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E10" s="8">
-        <v>200000</v>
+      <c r="B10" s="33"/>
+      <c r="C10" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="11" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E10" s="12" t="n">
+        <v>168600.0</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="20"/>
-      <c r="C11" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E11" s="10"/>
+      <c r="B11" s="20" t="n">
+        <v>2023.0</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E11" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="20"/>
-      <c r="C12" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="13">
-        <v>6.2</v>
-      </c>
-      <c r="E12" s="14">
-        <v>152000</v>
-      </c>
+      <c r="B12" s="32"/>
+      <c r="C12" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E12" s="10"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="20">
-        <v>2022</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E13" s="8">
-        <v>200000</v>
+      <c r="B13" s="31"/>
+      <c r="C13" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="13" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E13" s="14" t="n">
+        <v>152000.0</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="20"/>
-      <c r="C14" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E14" s="10"/>
+      <c r="B14" s="20" t="n">
+        <v>2022.0</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E14" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="20"/>
-      <c r="C15" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="11">
-        <v>6.2</v>
-      </c>
-      <c r="E15" s="12">
-        <v>147000</v>
-      </c>
+      <c r="B15" s="30"/>
+      <c r="C15" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E15" s="10"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="20">
-        <v>2021</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E16" s="8">
-        <v>200000</v>
+      <c r="B16" s="29"/>
+      <c r="C16" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="11" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E16" s="12" t="n">
+        <v>147000.0</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="20"/>
-      <c r="C17" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E17" s="10"/>
+      <c r="B17" s="20" t="n">
+        <v>2021.0</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E17" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="20"/>
-      <c r="C18" s="18" t="s">
+      <c r="B18" s="28"/>
+      <c r="C18" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19">
+      <c r="B19" s="27"/>
+      <c r="C19" t="s" s="18">
         <v>2</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D19" t="s" s="11">
         <v>3</v>
       </c>
-      <c r="E18" s="12">
-        <v>142800</v>
-      </c>
+      <c r="E19" t="n" s="12">
+        <v>142800.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" s="26"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="23"/>
     </row>
     <row r="1047484" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1047485" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1988,13 +2092,13 @@
     <row r="1048545" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1048546" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B16:B18"/>
+  <mergeCells count="11">
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B5:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
adding properties to table Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/CAP Financial/rules/config_financial_base.xlsx
+++ b/DESIGN/rules/CAP Financial/rules/config_financial_base.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="22">
   <si>
     <t>Fica Type</t>
   </si>
@@ -83,6 +83,15 @@
   </si>
   <si>
     <t>Rate</t>
+  </si>
+  <si>
+    <t>properties</t>
+  </si>
+  <si>
+    <t>origin</t>
+  </si>
+  <si>
+    <t>Deviation</t>
   </si>
 </sst>
 </file>
@@ -207,7 +216,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -445,12 +454,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -510,6 +561,41 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="true"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="true"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="true"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,198 +817,216 @@
       <c r="E2" s="21"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="B3" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="39"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="20">
-        <v>2025</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E4" s="8">
-        <v>200000</v>
+      <c r="B4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="20"/>
-      <c r="C5" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E5" s="10"/>
+      <c r="B5" s="20" t="n">
+        <v>2025.0</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E5" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="20"/>
-      <c r="C6" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="11">
-        <v>6.2</v>
-      </c>
-      <c r="E6" s="12">
-        <v>168600</v>
-      </c>
+      <c r="B6" s="36"/>
+      <c r="C6" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="20">
-        <v>2024</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E7" s="8">
-        <v>200000</v>
+      <c r="B7" s="35"/>
+      <c r="C7" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="11" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E7" s="12" t="n">
+        <v>168600.0</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="20"/>
-      <c r="C8" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E8" s="10"/>
+      <c r="B8" s="20" t="n">
+        <v>2024.0</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E8" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="20"/>
-      <c r="C9" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="11">
-        <v>6.2</v>
-      </c>
-      <c r="E9" s="12">
-        <v>168600</v>
-      </c>
+      <c r="B9" s="34"/>
+      <c r="C9" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E9" s="10"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="20">
-        <v>2023</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E10" s="8">
-        <v>200000</v>
+      <c r="B10" s="33"/>
+      <c r="C10" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="11" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E10" s="12" t="n">
+        <v>168600.0</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="20"/>
-      <c r="C11" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E11" s="10"/>
+      <c r="B11" s="20" t="n">
+        <v>2023.0</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E11" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="20"/>
-      <c r="C12" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="13">
-        <v>6.2</v>
-      </c>
-      <c r="E12" s="14">
-        <v>152000</v>
-      </c>
+      <c r="B12" s="32"/>
+      <c r="C12" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E12" s="10"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="20">
-        <v>2022</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E13" s="8">
-        <v>200000</v>
+      <c r="B13" s="31"/>
+      <c r="C13" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="13" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E13" s="14" t="n">
+        <v>152000.0</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="20"/>
-      <c r="C14" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E14" s="10"/>
+      <c r="B14" s="20" t="n">
+        <v>2022.0</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E14" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="20"/>
-      <c r="C15" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="11">
-        <v>6.2</v>
-      </c>
-      <c r="E15" s="12">
-        <v>147000</v>
-      </c>
+      <c r="B15" s="30"/>
+      <c r="C15" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E15" s="10"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="20">
-        <v>2021</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E16" s="8">
-        <v>200000</v>
+      <c r="B16" s="29"/>
+      <c r="C16" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="11" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E16" s="12" t="n">
+        <v>147000.0</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="20"/>
-      <c r="C17" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E17" s="10"/>
+      <c r="B17" s="20" t="n">
+        <v>2021.0</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E17" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="20"/>
-      <c r="C18" s="18" t="s">
+      <c r="B18" s="28"/>
+      <c r="C18" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19">
+      <c r="B19" s="27"/>
+      <c r="C19" t="s" s="18">
         <v>2</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D19" t="s" s="11">
         <v>3</v>
       </c>
-      <c r="E18" s="12">
-        <v>142800</v>
-      </c>
+      <c r="E19" t="n" s="12">
+        <v>142800.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" s="26"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="23"/>
     </row>
     <row r="1047484" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1047485" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1988,13 +2092,13 @@
     <row r="1048545" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1048546" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B16:B18"/>
+  <mergeCells count="11">
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B5:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
ABC-123: Added user login functionality Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/CAP Financial/rules/config_financial_base.xlsx
+++ b/DESIGN/rules/CAP Financial/rules/config_financial_base.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="23">
   <si>
     <t>Fica Type</t>
   </si>
@@ -847,7 +847,7 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="20" t="n">
-        <v>2025.0</v>
+        <v>2026.0</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>13</v>
@@ -861,7 +861,7 @@
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="36" t="n">
-        <v>2025.0</v>
+        <v>2026.0</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>14</v>
@@ -873,7 +873,7 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" s="35" t="n">
-        <v>2025.0</v>
+        <v>2026.0</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>2</v>
@@ -887,7 +887,7 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" s="20" t="n">
-        <v>2024.0</v>
+        <v>2025.0</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>13</v>
@@ -901,7 +901,7 @@
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B9" s="34" t="n">
-        <v>2024.0</v>
+        <v>2025.0</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>14</v>
@@ -913,13 +913,13 @@
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B10" s="33" t="n">
-        <v>2024.0</v>
+        <v>2025.0</v>
       </c>
       <c r="C10" s="18" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="11" t="n">
-        <v>6.2</v>
+        <v>6.3</v>
       </c>
       <c r="E10" s="12" t="n">
         <v>168600.0</v>
@@ -927,7 +927,7 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B11" s="20" t="n">
-        <v>2023.0</v>
+        <v>2024.0</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>13</v>
@@ -941,7 +941,7 @@
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B12" s="32" t="n">
-        <v>2023.0</v>
+        <v>2024.0</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>14</v>
@@ -953,7 +953,7 @@
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13" s="31" t="n">
-        <v>2023.0</v>
+        <v>2024.0</v>
       </c>
       <c r="C13" s="19" t="s">
         <v>2</v>
@@ -962,12 +962,12 @@
         <v>6.2</v>
       </c>
       <c r="E13" s="14" t="n">
-        <v>152000.0</v>
+        <v>168600.0</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B14" s="20" t="n">
-        <v>2022.0</v>
+        <v>2023.0</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>13</v>
@@ -981,7 +981,7 @@
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B15" s="30" t="n">
-        <v>2022.0</v>
+        <v>2023.0</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>14</v>
@@ -993,7 +993,7 @@
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B16" s="29" t="n">
-        <v>2022.0</v>
+        <v>2023.0</v>
       </c>
       <c r="C16" s="18" t="s">
         <v>2</v>
@@ -1002,12 +1002,12 @@
         <v>6.2</v>
       </c>
       <c r="E16" s="12" t="n">
-        <v>147000.0</v>
+        <v>152000.0</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="20" t="n">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>13</v>
@@ -1021,7 +1021,7 @@
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" s="28" t="n">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>14</v>
@@ -1033,7 +1033,7 @@
     </row>
     <row r="19">
       <c r="B19" s="27" t="n">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="C19" s="18" t="s">
         <v>2</v>
@@ -1042,14 +1042,54 @@
         <v>6.2</v>
       </c>
       <c r="E19" t="n" s="12">
-        <v>142800.0</v>
+        <v>147000.0</v>
       </c>
     </row>
     <row r="20">
-      <c r="B20" s="26"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="23"/>
+      <c r="B20" t="n" s="5">
+        <v>2021.0</v>
+      </c>
+      <c r="C20" t="s" s="5">
+        <v>13</v>
+      </c>
+      <c r="D20" t="n" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="E20" t="n" s="5">
+        <v>200000.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="n" s="5">
+        <v>2021.0</v>
+      </c>
+      <c r="C21" t="s" s="5">
+        <v>14</v>
+      </c>
+      <c r="D21" t="n" s="5">
+        <v>1.45</v>
+      </c>
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22">
+      <c r="B22" t="n" s="5">
+        <v>2021.0</v>
+      </c>
+      <c r="C22" t="s" s="5">
+        <v>2</v>
+      </c>
+      <c r="D22" t="n" s="5">
+        <v>6.2</v>
+      </c>
+      <c r="E22" t="n" s="5">
+        <v>142800.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" s="5"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
     </row>
     <row r="1047484" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1047485" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
GLIC -12 Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/CAP Financial/rules/config_financial_base.xlsx
+++ b/DESIGN/rules/CAP Financial/rules/config_financial_base.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="23">
   <si>
     <t>Fica Type</t>
   </si>
@@ -847,7 +847,7 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="20" t="n">
-        <v>2026.0</v>
+        <v>2027.0</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>13</v>
@@ -861,7 +861,7 @@
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="36" t="n">
-        <v>2026.0</v>
+        <v>2027.0</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>14</v>
@@ -873,7 +873,7 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" s="35" t="n">
-        <v>2026.0</v>
+        <v>2027.0</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>2</v>
@@ -887,7 +887,7 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" s="20" t="n">
-        <v>2025.0</v>
+        <v>2026.0</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>13</v>
@@ -901,7 +901,7 @@
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B9" s="34" t="n">
-        <v>2025.0</v>
+        <v>2026.0</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>14</v>
@@ -913,7 +913,7 @@
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B10" s="33" t="n">
-        <v>2025.0</v>
+        <v>2026.0</v>
       </c>
       <c r="C10" s="18" t="s">
         <v>2</v>
@@ -927,7 +927,7 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B11" s="20" t="n">
-        <v>2024.0</v>
+        <v>2025.0</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>13</v>
@@ -941,7 +941,7 @@
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B12" s="32" t="n">
-        <v>2024.0</v>
+        <v>2025.0</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>14</v>
@@ -953,13 +953,13 @@
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13" s="31" t="n">
-        <v>2024.0</v>
+        <v>2025.0</v>
       </c>
       <c r="C13" s="19" t="s">
         <v>2</v>
       </c>
       <c r="D13" s="13" t="n">
-        <v>6.2</v>
+        <v>6.3</v>
       </c>
       <c r="E13" s="14" t="n">
         <v>168600.0</v>
@@ -967,7 +967,7 @@
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B14" s="20" t="n">
-        <v>2023.0</v>
+        <v>2024.0</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>13</v>
@@ -981,7 +981,7 @@
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B15" s="30" t="n">
-        <v>2023.0</v>
+        <v>2024.0</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>14</v>
@@ -993,7 +993,7 @@
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B16" s="29" t="n">
-        <v>2023.0</v>
+        <v>2024.0</v>
       </c>
       <c r="C16" s="18" t="s">
         <v>2</v>
@@ -1002,12 +1002,12 @@
         <v>6.2</v>
       </c>
       <c r="E16" s="12" t="n">
-        <v>152000.0</v>
+        <v>168600.0</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="20" t="n">
-        <v>2022.0</v>
+        <v>2023.0</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>13</v>
@@ -1021,7 +1021,7 @@
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" s="28" t="n">
-        <v>2022.0</v>
+        <v>2023.0</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>14</v>
@@ -1033,7 +1033,7 @@
     </row>
     <row r="19">
       <c r="B19" s="27" t="n">
-        <v>2022.0</v>
+        <v>2023.0</v>
       </c>
       <c r="C19" s="18" t="s">
         <v>2</v>
@@ -1042,14 +1042,14 @@
         <v>6.2</v>
       </c>
       <c r="E19" t="n" s="12">
-        <v>147000.0</v>
+        <v>152000.0</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="n" s="5">
-        <v>2021.0</v>
-      </c>
-      <c r="C20" t="s" s="5">
+        <v>2022.0</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D20" t="n" s="5">
@@ -1061,9 +1061,9 @@
     </row>
     <row r="21">
       <c r="B21" t="n" s="5">
-        <v>2021.0</v>
-      </c>
-      <c r="C21" t="s" s="5">
+        <v>2022.0</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D21" t="n" s="5">
@@ -1073,23 +1073,63 @@
     </row>
     <row r="22">
       <c r="B22" t="n" s="5">
-        <v>2021.0</v>
-      </c>
-      <c r="C22" t="s" s="5">
+        <v>2022.0</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D22" t="n" s="5">
         <v>6.2</v>
       </c>
       <c r="E22" t="n" s="5">
-        <v>142800.0</v>
+        <v>147000.0</v>
       </c>
     </row>
     <row r="23">
-      <c r="B23" s="5"/>
-      <c r="C23"/>
-      <c r="D23"/>
-      <c r="E23"/>
+      <c r="B23" t="n" s="5">
+        <v>2021.0</v>
+      </c>
+      <c r="C23" t="s" s="5">
+        <v>13</v>
+      </c>
+      <c r="D23" t="n" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="E23" t="n" s="5">
+        <v>200000.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="n" s="5">
+        <v>2021.0</v>
+      </c>
+      <c r="C24" t="s" s="5">
+        <v>14</v>
+      </c>
+      <c r="D24" t="n" s="5">
+        <v>1.45</v>
+      </c>
+      <c r="E24" s="5"/>
+    </row>
+    <row r="25">
+      <c r="B25" t="n" s="5">
+        <v>2021.0</v>
+      </c>
+      <c r="C25" t="s" s="5">
+        <v>2</v>
+      </c>
+      <c r="D25" t="n" s="5">
+        <v>6.2</v>
+      </c>
+      <c r="E25" t="n" s="5">
+        <v>142800.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" s="5"/>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26"/>
     </row>
     <row r="1047484" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1047485" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
TEST - Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/CAP Financial/rules/config_financial_base.xlsx
+++ b/DESIGN/rules/CAP Financial/rules/config_financial_base.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="23">
   <si>
     <t>Fica Type</t>
   </si>
@@ -847,7 +847,7 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="20" t="n">
-        <v>2027.0</v>
+        <v>2028.0</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>13</v>
@@ -861,7 +861,7 @@
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="36" t="n">
-        <v>2027.0</v>
+        <v>2028.0</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>14</v>
@@ -873,7 +873,7 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" s="35" t="n">
-        <v>2027.0</v>
+        <v>2028.0</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>2</v>
@@ -887,13 +887,13 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" s="20" t="n">
-        <v>2026.0</v>
+        <v>2027.0</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="15" t="n">
-        <v>0.9</v>
+        <v>0.93</v>
       </c>
       <c r="E8" s="8" t="n">
         <v>200000.0</v>
@@ -901,25 +901,25 @@
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B9" s="34" t="n">
-        <v>2026.0</v>
+        <v>2027.0</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="9" t="n">
-        <v>1.45</v>
+        <v>1.454</v>
       </c>
       <c r="E9" s="10"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B10" s="33" t="n">
-        <v>2026.0</v>
+        <v>2027.0</v>
       </c>
       <c r="C10" s="18" t="s">
         <v>2</v>
       </c>
       <c r="D10" s="11" t="n">
-        <v>6.3</v>
+        <v>6.4</v>
       </c>
       <c r="E10" s="12" t="n">
         <v>168600.0</v>
@@ -927,7 +927,7 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B11" s="20" t="n">
-        <v>2025.0</v>
+        <v>2026.0</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>13</v>
@@ -941,7 +941,7 @@
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B12" s="32" t="n">
-        <v>2025.0</v>
+        <v>2026.0</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>14</v>
@@ -953,7 +953,7 @@
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13" s="31" t="n">
-        <v>2025.0</v>
+        <v>2026.0</v>
       </c>
       <c r="C13" s="19" t="s">
         <v>2</v>
@@ -967,7 +967,7 @@
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B14" s="20" t="n">
-        <v>2024.0</v>
+        <v>2025.0</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>13</v>
@@ -981,7 +981,7 @@
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B15" s="30" t="n">
-        <v>2024.0</v>
+        <v>2025.0</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>14</v>
@@ -993,13 +993,13 @@
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B16" s="29" t="n">
-        <v>2024.0</v>
+        <v>2025.0</v>
       </c>
       <c r="C16" s="18" t="s">
         <v>2</v>
       </c>
       <c r="D16" s="11" t="n">
-        <v>6.2</v>
+        <v>6.3</v>
       </c>
       <c r="E16" s="12" t="n">
         <v>168600.0</v>
@@ -1007,7 +1007,7 @@
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="20" t="n">
-        <v>2023.0</v>
+        <v>2024.0</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>13</v>
@@ -1021,7 +1021,7 @@
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" s="28" t="n">
-        <v>2023.0</v>
+        <v>2024.0</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>14</v>
@@ -1033,7 +1033,7 @@
     </row>
     <row r="19">
       <c r="B19" s="27" t="n">
-        <v>2023.0</v>
+        <v>2024.0</v>
       </c>
       <c r="C19" s="18" t="s">
         <v>2</v>
@@ -1042,12 +1042,12 @@
         <v>6.2</v>
       </c>
       <c r="E19" t="n" s="12">
-        <v>152000.0</v>
+        <v>168600.0</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="n" s="5">
-        <v>2022.0</v>
+        <v>2023.0</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>13</v>
@@ -1061,7 +1061,7 @@
     </row>
     <row r="21">
       <c r="B21" t="n" s="5">
-        <v>2022.0</v>
+        <v>2023.0</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>14</v>
@@ -1073,7 +1073,7 @@
     </row>
     <row r="22">
       <c r="B22" t="n" s="5">
-        <v>2022.0</v>
+        <v>2023.0</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>2</v>
@@ -1082,12 +1082,12 @@
         <v>6.2</v>
       </c>
       <c r="E22" t="n" s="5">
-        <v>147000.0</v>
+        <v>152000.0</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="n" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>13</v>
@@ -1101,7 +1101,7 @@
     </row>
     <row r="24">
       <c r="B24" t="n" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>14</v>
@@ -1113,7 +1113,7 @@
     </row>
     <row r="25">
       <c r="B25" t="n" s="5">
-        <v>2021.0</v>
+        <v>2022.0</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>2</v>
@@ -1122,14 +1122,54 @@
         <v>6.2</v>
       </c>
       <c r="E25" t="n" s="5">
-        <v>142800.0</v>
+        <v>147000.0</v>
       </c>
     </row>
     <row r="26">
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
+      <c r="B26" t="n" s="5">
+        <v>2021.0</v>
+      </c>
+      <c r="C26" t="s" s="5">
+        <v>13</v>
+      </c>
+      <c r="D26" t="n" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="E26" t="n" s="5">
+        <v>200000.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="n" s="5">
+        <v>2021.0</v>
+      </c>
+      <c r="C27" t="s" s="5">
+        <v>14</v>
+      </c>
+      <c r="D27" t="n" s="5">
+        <v>1.45</v>
+      </c>
+      <c r="E27" s="5"/>
+    </row>
+    <row r="28">
+      <c r="B28" t="n" s="5">
+        <v>2021.0</v>
+      </c>
+      <c r="C28" t="s" s="5">
+        <v>2</v>
+      </c>
+      <c r="D28" t="n" s="5">
+        <v>6.2</v>
+      </c>
+      <c r="E28" t="n" s="5">
+        <v>142800.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" s="5"/>
+      <c r="C29"/>
+      <c r="D29"/>
+      <c r="E29"/>
     </row>
     <row r="1047484" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1047485" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
creating properties Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/CAP Financial/rules/config_financial_base.xlsx
+++ b/DESIGN/rules/CAP Financial/rules/config_financial_base.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="22">
   <si>
     <t>Fica Type</t>
   </si>
@@ -83,6 +83,15 @@
   </si>
   <si>
     <t>Rate</t>
+  </si>
+  <si>
+    <t>properties</t>
+  </si>
+  <si>
+    <t>origin</t>
+  </si>
+  <si>
+    <t>Deviation</t>
   </si>
 </sst>
 </file>
@@ -207,7 +216,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -445,12 +454,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -510,6 +561,41 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="true"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="true"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="true"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,198 +817,216 @@
       <c r="E2" s="21"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="B3" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="39"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="20">
-        <v>2025</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E4" s="8">
-        <v>200000</v>
+      <c r="B4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="20"/>
-      <c r="C5" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E5" s="10"/>
+      <c r="B5" s="20" t="n">
+        <v>2025.0</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E5" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="20"/>
-      <c r="C6" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="11">
-        <v>6.2</v>
-      </c>
-      <c r="E6" s="12">
-        <v>168600</v>
-      </c>
+      <c r="B6" s="36"/>
+      <c r="C6" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="20">
-        <v>2024</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E7" s="8">
-        <v>200000</v>
+      <c r="B7" s="35"/>
+      <c r="C7" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="11" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E7" s="12" t="n">
+        <v>168600.0</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="20"/>
-      <c r="C8" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E8" s="10"/>
+      <c r="B8" s="20" t="n">
+        <v>2024.0</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E8" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="20"/>
-      <c r="C9" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="11">
-        <v>6.2</v>
-      </c>
-      <c r="E9" s="12">
-        <v>168600</v>
-      </c>
+      <c r="B9" s="34"/>
+      <c r="C9" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E9" s="10"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="20">
-        <v>2023</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E10" s="8">
-        <v>200000</v>
+      <c r="B10" s="33"/>
+      <c r="C10" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="11" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E10" s="12" t="n">
+        <v>168600.0</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="20"/>
-      <c r="C11" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E11" s="10"/>
+      <c r="B11" s="20" t="n">
+        <v>2023.0</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E11" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="20"/>
-      <c r="C12" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="13">
-        <v>6.2</v>
-      </c>
-      <c r="E12" s="14">
-        <v>152000</v>
-      </c>
+      <c r="B12" s="32"/>
+      <c r="C12" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E12" s="10"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="20">
-        <v>2022</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E13" s="8">
-        <v>200000</v>
+      <c r="B13" s="31"/>
+      <c r="C13" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="13" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E13" s="14" t="n">
+        <v>152000.0</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="20"/>
-      <c r="C14" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E14" s="10"/>
+      <c r="B14" s="20" t="n">
+        <v>2022.0</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E14" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="20"/>
-      <c r="C15" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="11">
-        <v>6.2</v>
-      </c>
-      <c r="E15" s="12">
-        <v>147000</v>
-      </c>
+      <c r="B15" s="30"/>
+      <c r="C15" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E15" s="10"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="20">
-        <v>2021</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E16" s="8">
-        <v>200000</v>
+      <c r="B16" s="29"/>
+      <c r="C16" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="11" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E16" s="12" t="n">
+        <v>147000.0</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="20"/>
-      <c r="C17" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E17" s="10"/>
+      <c r="B17" s="20" t="n">
+        <v>2021.0</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E17" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="20"/>
-      <c r="C18" s="18" t="s">
+      <c r="B18" s="28"/>
+      <c r="C18" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19">
+      <c r="B19" s="27"/>
+      <c r="C19" t="s" s="18">
         <v>2</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D19" t="s" s="11">
         <v>3</v>
       </c>
-      <c r="E18" s="12">
-        <v>142800</v>
-      </c>
+      <c r="E19" t="n" s="12">
+        <v>142800.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" s="26"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="23"/>
     </row>
     <row r="1047484" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1047485" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1988,13 +2092,13 @@
     <row r="1048545" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1048546" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B16:B18"/>
+  <mergeCells count="11">
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B5:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
BUG-456: Resolved issue with payment gateway integration Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/CAP Financial/rules/config_financial_base.xlsx
+++ b/DESIGN/rules/CAP Financial/rules/config_financial_base.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="23">
   <si>
     <t>Fica Type</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>Deviation</t>
+  </si>
+  <si>
+    <t>SmartRules PaymentToolsFicaDetails FicaTaxRates(PaymentToolsFicaInput input)</t>
   </si>
 </sst>
 </file>
@@ -828,7 +831,7 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B2" s="21" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C2" s="21"/>
       <c r="D2" s="21"/>
@@ -862,35 +865,39 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" s="20" t="n">
-        <v>2025.0</v>
+        <v>2026.0</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="15" t="n">
-        <v>0.9</v>
+        <v>0.92</v>
       </c>
       <c r="E5" s="8" t="n">
-        <v>200000.0</v>
+        <v>200.0</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="36"/>
+      <c r="B6" s="36" t="n">
+        <v>2026.0</v>
+      </c>
       <c r="C6" s="17" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="9" t="n">
-        <v>1.453</v>
+        <v>1.45</v>
       </c>
       <c r="E6" s="10"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="35"/>
+      <c r="B7" s="35" t="n">
+        <v>2026.0</v>
+      </c>
       <c r="C7" s="18" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="11" t="n">
-        <v>6.2</v>
+        <v>6.3</v>
       </c>
       <c r="E7" s="12" t="n">
         <v>168600.0</v>
@@ -898,30 +905,34 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" s="20" t="n">
-        <v>2026.0</v>
+        <v>2025.0</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="15" t="n">
-        <v>0.92</v>
+        <v>0.9</v>
       </c>
       <c r="E8" s="8" t="n">
-        <v>200.0</v>
+        <v>200000.0</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="36"/>
+      <c r="B9" s="36" t="n">
+        <v>2025.0</v>
+      </c>
       <c r="C9" s="17" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="9" t="n">
-        <v>1.45</v>
+        <v>1.453</v>
       </c>
       <c r="E9" s="10"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="35"/>
+      <c r="B10" s="35" t="n">
+        <v>2025.0</v>
+      </c>
       <c r="C10" s="18" t="s">
         <v>2</v>
       </c>
@@ -947,7 +958,9 @@
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="47"/>
+      <c r="B12" s="47" t="n">
+        <v>2024.0</v>
+      </c>
       <c r="C12" s="17" t="s">
         <v>14</v>
       </c>
@@ -957,7 +970,9 @@
       <c r="E12" s="10"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="46"/>
+      <c r="B13" s="46" t="n">
+        <v>2024.0</v>
+      </c>
       <c r="C13" s="18" t="s">
         <v>2</v>
       </c>
@@ -983,7 +998,9 @@
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="45"/>
+      <c r="B15" s="45" t="n">
+        <v>2023.0</v>
+      </c>
       <c r="C15" s="17" t="s">
         <v>14</v>
       </c>
@@ -993,7 +1010,9 @@
       <c r="E15" s="10"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="44"/>
+      <c r="B16" s="44" t="n">
+        <v>2023.0</v>
+      </c>
       <c r="C16" s="19" t="s">
         <v>2</v>
       </c>
@@ -1019,7 +1038,9 @@
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="43"/>
+      <c r="B18" s="43" t="n">
+        <v>2022.0</v>
+      </c>
       <c r="C18" s="17" t="s">
         <v>14</v>
       </c>
@@ -1029,7 +1050,9 @@
       <c r="E18" s="10"/>
     </row>
     <row r="19">
-      <c r="B19" s="42"/>
+      <c r="B19" s="42" t="n">
+        <v>2022.0</v>
+      </c>
       <c r="C19" s="18" t="s">
         <v>2</v>
       </c>
@@ -1044,7 +1067,7 @@
       <c r="B20" t="n" s="20">
         <v>2021.0</v>
       </c>
-      <c r="C20" t="s" s="16">
+      <c r="C20" s="16" t="s">
         <v>13</v>
       </c>
       <c r="D20" t="n" s="15">
@@ -1055,8 +1078,10 @@
       </c>
     </row>
     <row r="21">
-      <c r="B21" s="41"/>
-      <c r="C21" t="s" s="17">
+      <c r="B21" s="41" t="n">
+        <v>2021.0</v>
+      </c>
+      <c r="C21" s="17" t="s">
         <v>14</v>
       </c>
       <c r="D21" t="n" s="9">
@@ -1065,12 +1090,14 @@
       <c r="E21" s="10"/>
     </row>
     <row r="22">
-      <c r="B22" s="40"/>
-      <c r="C22" t="s" s="18">
+      <c r="B22" s="40" t="n">
+        <v>2021.0</v>
+      </c>
+      <c r="C22" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D22" t="s" s="11">
-        <v>3</v>
+      <c r="D22" t="n" s="11">
+        <v>6.2</v>
       </c>
       <c r="E22" t="n" s="12">
         <v>142800.0</v>

</xml_diff>

<commit_message>
set properties Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/CAP Financial/rules/config_financial_base.xlsx
+++ b/DESIGN/rules/CAP Financial/rules/config_financial_base.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="22">
   <si>
     <t>Fica Type</t>
   </si>
@@ -83,6 +83,15 @@
   </si>
   <si>
     <t>Rate</t>
+  </si>
+  <si>
+    <t>properties</t>
+  </si>
+  <si>
+    <t>origin</t>
+  </si>
+  <si>
+    <t>Deviation</t>
   </si>
 </sst>
 </file>
@@ -207,7 +216,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -445,12 +454,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -510,6 +561,41 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="true"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="true" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="true"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="true"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,198 +817,216 @@
       <c r="E2" s="21"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="B3" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="39"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="20">
-        <v>2025</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E4" s="8">
-        <v>200000</v>
+      <c r="B4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="20"/>
-      <c r="C5" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E5" s="10"/>
+      <c r="B5" s="20" t="n">
+        <v>2025.0</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E5" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="20"/>
-      <c r="C6" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="11">
-        <v>6.2</v>
-      </c>
-      <c r="E6" s="12">
-        <v>168600</v>
-      </c>
+      <c r="B6" s="36"/>
+      <c r="C6" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="20">
-        <v>2024</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E7" s="8">
-        <v>200000</v>
+      <c r="B7" s="35"/>
+      <c r="C7" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="11" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E7" s="12" t="n">
+        <v>168600.0</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="20"/>
-      <c r="C8" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E8" s="10"/>
+      <c r="B8" s="20" t="n">
+        <v>2024.0</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E8" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="20"/>
-      <c r="C9" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="11">
-        <v>6.2</v>
-      </c>
-      <c r="E9" s="12">
-        <v>168600</v>
-      </c>
+      <c r="B9" s="34"/>
+      <c r="C9" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E9" s="10"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="20">
-        <v>2023</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E10" s="8">
-        <v>200000</v>
+      <c r="B10" s="33"/>
+      <c r="C10" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="11" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E10" s="12" t="n">
+        <v>168600.0</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="20"/>
-      <c r="C11" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E11" s="10"/>
+      <c r="B11" s="20" t="n">
+        <v>2023.0</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E11" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="20"/>
-      <c r="C12" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="13">
-        <v>6.2</v>
-      </c>
-      <c r="E12" s="14">
-        <v>152000</v>
-      </c>
+      <c r="B12" s="32"/>
+      <c r="C12" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E12" s="10"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="20">
-        <v>2022</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E13" s="8">
-        <v>200000</v>
+      <c r="B13" s="31"/>
+      <c r="C13" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="13" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E13" s="14" t="n">
+        <v>152000.0</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="20"/>
-      <c r="C14" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E14" s="10"/>
+      <c r="B14" s="20" t="n">
+        <v>2022.0</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E14" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="20"/>
-      <c r="C15" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="11">
-        <v>6.2</v>
-      </c>
-      <c r="E15" s="12">
-        <v>147000</v>
-      </c>
+      <c r="B15" s="30"/>
+      <c r="C15" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E15" s="10"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="20">
-        <v>2021</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="15">
-        <v>0.9</v>
-      </c>
-      <c r="E16" s="8">
-        <v>200000</v>
+      <c r="B16" s="29"/>
+      <c r="C16" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="11" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="E16" s="12" t="n">
+        <v>147000.0</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="20"/>
-      <c r="C17" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="9">
-        <v>1.45</v>
-      </c>
-      <c r="E17" s="10"/>
+      <c r="B17" s="20" t="n">
+        <v>2021.0</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E17" s="8" t="n">
+        <v>200000.0</v>
+      </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="20"/>
-      <c r="C18" s="18" t="s">
+      <c r="B18" s="28"/>
+      <c r="C18" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="9" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19">
+      <c r="B19" s="27"/>
+      <c r="C19" t="s" s="18">
         <v>2</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D19" t="s" s="11">
         <v>3</v>
       </c>
-      <c r="E18" s="12">
-        <v>142800</v>
-      </c>
+      <c r="E19" t="n" s="12">
+        <v>142800.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" s="26"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="23"/>
     </row>
     <row r="1047484" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1047485" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1988,13 +2092,13 @@
     <row r="1048545" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1048546" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B16:B18"/>
+  <mergeCells count="11">
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B5:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="landscape" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>